<commit_message>
re-running all the data summarization and cleaning code, because I redesignated the "background" and "treatment" variables as the same in the F0 generation.
</commit_message>
<xml_diff>
--- a/raw_data/performance_data.xlsx
+++ b/raw_data/performance_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E407CC-1EE5-2144-B6BD-06695BAC74A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD1C96-7395-DE4B-A487-C6EA19F9BD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32420" yWindow="500" windowWidth="32420" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="637">
   <si>
     <t>ind_id</t>
   </si>
@@ -1930,6 +1930,21 @@
   <si>
     <t>F3_076_DEV</t>
   </si>
+  <si>
+    <t>L4_E</t>
+  </si>
+  <si>
+    <t>L7_E</t>
+  </si>
+  <si>
+    <t>L11_E</t>
+  </si>
+  <si>
+    <t>L12_E</t>
+  </si>
+  <si>
+    <t>L9_E</t>
+  </si>
 </sst>
 </file>
 
@@ -2356,9 +2371,9 @@
   </sheetPr>
   <dimension ref="A1:BJ997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BH189" sqref="BH189"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2:E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2757,7 +2772,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>63</v>
+        <v>343</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>64</v>
@@ -3125,7 +3140,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>76</v>
+        <v>632</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>64</v>
@@ -3861,7 +3876,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>64</v>
@@ -4049,7 +4064,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>64</v>
@@ -4237,7 +4252,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>64</v>
@@ -4801,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>64</v>
@@ -4989,7 +5004,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>64</v>
@@ -5177,7 +5192,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>64</v>
@@ -5349,7 +5364,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>64</v>
@@ -5717,7 +5732,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>64</v>
@@ -6093,7 +6108,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>64</v>
@@ -6281,7 +6296,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>64</v>
@@ -6845,7 +6860,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>64</v>
@@ -7033,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>64</v>
@@ -7575,7 +7590,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>64</v>
@@ -7935,7 +7950,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>64</v>
@@ -8123,7 +8138,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>64</v>
@@ -8303,7 +8318,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>64</v>
@@ -8491,7 +8506,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>76</v>
+        <v>632</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>64</v>
@@ -8843,7 +8858,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>64</v>
@@ -9015,7 +9030,7 @@
         <v>6</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>64</v>
@@ -9753,7 +9768,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>64</v>
@@ -10505,7 +10520,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>64</v>
@@ -11225,7 +11240,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>76</v>
+        <v>632</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>64</v>
@@ -12133,7 +12148,7 @@
         <v>5</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>64</v>
@@ -12313,7 +12328,7 @@
         <v>6</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>64</v>
@@ -12485,7 +12500,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>64</v>
@@ -13221,7 +13236,7 @@
         <v>5</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>64</v>
@@ -13753,7 +13768,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>64</v>
@@ -14115,7 +14130,7 @@
         <v>4</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>64</v>
@@ -14475,7 +14490,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>64</v>
@@ -14851,7 +14866,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>64</v>
@@ -15415,7 +15430,7 @@
         <v>5</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>63</v>
+        <v>343</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>64</v>
@@ -15971,7 +15986,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>63</v>
+        <v>343</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>64</v>
@@ -16143,7 +16158,7 @@
         <v>3</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>63</v>
+        <v>343</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>64</v>
@@ -16331,7 +16346,7 @@
         <v>4</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>64</v>
@@ -16519,7 +16534,7 @@
         <v>5</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>64</v>
@@ -17083,7 +17098,7 @@
         <v>2</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>64</v>
@@ -17271,7 +17286,7 @@
         <v>3</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="F82" s="8" t="s">
         <v>64</v>
@@ -17459,7 +17474,7 @@
         <v>2</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>64</v>
@@ -17647,7 +17662,7 @@
         <v>4</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>63</v>
+        <v>343</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>64</v>
@@ -17999,7 +18014,7 @@
         <v>1</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>64</v>
@@ -18187,7 +18202,7 @@
         <v>2</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>64</v>
@@ -18547,7 +18562,7 @@
         <v>4</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>64</v>
@@ -18735,7 +18750,7 @@
         <v>5</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>64</v>
@@ -19487,7 +19502,7 @@
         <v>3</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>64</v>
@@ -19659,7 +19674,7 @@
         <v>4</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>64</v>
@@ -19847,7 +19862,7 @@
         <v>5</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>64</v>
@@ -20393,7 +20408,7 @@
         <v>2</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>76</v>
+        <v>632</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>64</v>
@@ -20581,7 +20596,7 @@
         <v>3</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="F100" s="8" t="s">
         <v>64</v>
@@ -20753,7 +20768,7 @@
         <v>4</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>76</v>
+        <v>632</v>
       </c>
       <c r="F101" s="8" t="s">
         <v>64</v>
@@ -21317,7 +21332,7 @@
         <v>1</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="F104" s="8" t="s">
         <v>64</v>
@@ -21677,7 +21692,7 @@
         <v>3</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>63</v>
+        <v>343</v>
       </c>
       <c r="F106" s="8" t="s">
         <v>64</v>
@@ -21865,7 +21880,7 @@
         <v>4</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>76</v>
+        <v>632</v>
       </c>
       <c r="F107" s="8" t="s">
         <v>64</v>
@@ -22413,7 +22428,7 @@
         <v>1</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="F110" s="8" t="s">
         <v>64</v>
@@ -22789,7 +22804,7 @@
         <v>3</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>296</v>
+        <v>635</v>
       </c>
       <c r="F112" s="8" t="s">
         <v>64</v>
@@ -23149,7 +23164,7 @@
         <v>5</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="F114" s="8" t="s">
         <v>64</v>
@@ -23525,7 +23540,7 @@
         <v>4</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>296</v>
+        <v>635</v>
       </c>
       <c r="F116" s="8" t="s">
         <v>64</v>
@@ -24457,7 +24472,7 @@
         <v>4</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="F121" s="8" t="s">
         <v>64</v>
@@ -24629,7 +24644,7 @@
         <v>5</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="F122" s="8" t="s">
         <v>64</v>
@@ -24817,7 +24832,7 @@
         <v>6</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>296</v>
+        <v>635</v>
       </c>
       <c r="F123" s="8" t="s">
         <v>64</v>
@@ -25005,7 +25020,7 @@
         <v>1</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>296</v>
+        <v>635</v>
       </c>
       <c r="F124" s="8" t="s">
         <v>64</v>
@@ -25373,7 +25388,7 @@
         <v>3</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="F126" s="8" t="s">
         <v>64</v>
@@ -25735,7 +25750,7 @@
         <v>5</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>296</v>
+        <v>635</v>
       </c>
       <c r="F128" s="8" t="s">
         <v>64</v>
@@ -25923,7 +25938,7 @@
         <v>6</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="F129" s="8" t="s">
         <v>64</v>
@@ -26447,7 +26462,7 @@
         <v>5</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>296</v>
+        <v>635</v>
       </c>
       <c r="F132" s="8" t="s">
         <v>64</v>
@@ -26791,7 +26806,7 @@
         <v>1</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F134" s="8" t="s">
         <v>64</v>
@@ -27519,7 +27534,7 @@
         <v>5</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F138" s="8" t="s">
         <v>64</v>
@@ -27691,7 +27706,7 @@
         <v>6</v>
       </c>
       <c r="E139" s="8" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F139" s="8" t="s">
         <v>64</v>
@@ -28247,7 +28262,7 @@
         <v>3</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F142" s="8" t="s">
         <v>64</v>
@@ -28419,7 +28434,7 @@
         <v>4</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F143" s="8" t="s">
         <v>64</v>
@@ -28591,7 +28606,7 @@
         <v>5</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F144" s="8" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
update to factor names and tried to fit distributions
</commit_message>
<xml_diff>
--- a/raw_data/performance_data.xlsx
+++ b/raw_data/performance_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE4873-415F-E94F-A3BF-CEB78F7CD612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055921EA-FF6E-1047-9664-9A9BEA19F0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2058,52 +2058,52 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2328,7 +2328,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J12" sqref="J12:J13"/>
+      <selection pane="topRight" activeCell="I2" sqref="I2:I145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2746,7 +2746,7 @@
         <v>70</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J3" s="11">
         <v>10</v>
@@ -3120,7 +3120,7 @@
         <v>70</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J5" s="11">
         <v>10</v>
@@ -3868,7 +3868,7 @@
         <v>70</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J9" s="11">
         <v>10</v>
@@ -4059,7 +4059,7 @@
         <v>70</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J10" s="11">
         <v>10</v>
@@ -4250,7 +4250,7 @@
         <v>70</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J11" s="11">
         <v>10</v>
@@ -4823,7 +4823,7 @@
         <v>70</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J14" s="11">
         <v>10</v>
@@ -5014,7 +5014,7 @@
         <v>70</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J15" s="11">
         <v>10</v>
@@ -5205,7 +5205,7 @@
         <v>70</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J16" s="11">
         <v>10</v>
@@ -5380,7 +5380,7 @@
         <v>70</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J17" s="11">
         <v>10</v>
@@ -5754,7 +5754,7 @@
         <v>70</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J19" s="11">
         <v>10</v>
@@ -6136,7 +6136,7 @@
         <v>70</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J21" s="11">
         <v>10</v>
@@ -6327,7 +6327,7 @@
         <v>70</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J22" s="11">
         <v>10</v>
@@ -6900,7 +6900,7 @@
         <v>70</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J25" s="11">
         <v>10</v>
@@ -7091,7 +7091,7 @@
         <v>70</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J26" s="11">
         <v>10</v>
@@ -7642,7 +7642,7 @@
         <v>70</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J29" s="11">
         <v>10</v>
@@ -8008,7 +8008,7 @@
         <v>70</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J31" s="11">
         <v>10</v>
@@ -8199,7 +8199,7 @@
         <v>70</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J32" s="11">
         <v>10</v>
@@ -8382,7 +8382,7 @@
         <v>70</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J33" s="11">
         <v>10</v>
@@ -8573,7 +8573,7 @@
         <v>70</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J34" s="11">
         <v>10</v>
@@ -8931,7 +8931,7 @@
         <v>70</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J36" s="11">
         <v>10</v>
@@ -9106,7 +9106,7 @@
         <v>70</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J37" s="11">
         <v>10</v>
@@ -9856,7 +9856,7 @@
         <v>70</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J41" s="11">
         <v>10</v>
@@ -10620,7 +10620,7 @@
         <v>70</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J45" s="11">
         <v>10</v>
@@ -11352,7 +11352,7 @@
         <v>70</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J49" s="11">
         <v>10</v>
@@ -12275,7 +12275,7 @@
         <v>70</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J54" s="11">
         <v>10</v>
@@ -12458,7 +12458,7 @@
         <v>70</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J55" s="11">
         <v>10</v>
@@ -12633,7 +12633,7 @@
         <v>70</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J56" s="11">
         <v>10</v>
@@ -13381,7 +13381,7 @@
         <v>70</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J60" s="11">
         <v>10</v>
@@ -13922,7 +13922,7 @@
         <v>70</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J63" s="11">
         <v>10</v>
@@ -14290,7 +14290,7 @@
         <v>70</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J65" s="11">
         <v>10</v>
@@ -14656,7 +14656,7 @@
         <v>70</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J67" s="11">
         <v>10</v>
@@ -15038,7 +15038,7 @@
         <v>70</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J69" s="11">
         <v>10</v>
@@ -15611,7 +15611,7 @@
         <v>70</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J72" s="11">
         <v>10</v>
@@ -16176,7 +16176,7 @@
         <v>70</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J75" s="11">
         <v>10</v>
@@ -16351,7 +16351,7 @@
         <v>70</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J76" s="11">
         <v>10</v>
@@ -16542,7 +16542,7 @@
         <v>70</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J77" s="11">
         <v>10</v>
@@ -16733,7 +16733,7 @@
         <v>70</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J78" s="11">
         <v>10</v>
@@ -17306,7 +17306,7 @@
         <v>70</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J81" s="11">
         <v>10</v>
@@ -17497,7 +17497,7 @@
         <v>70</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J82" s="11">
         <v>10</v>
@@ -17688,7 +17688,7 @@
         <v>70</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J83" s="11">
         <v>10</v>
@@ -17879,7 +17879,7 @@
         <v>70</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J84" s="11">
         <v>10</v>
@@ -18237,7 +18237,7 @@
         <v>70</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J86" s="11">
         <v>10</v>
@@ -18428,7 +18428,7 @@
         <v>70</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J87" s="11">
         <v>10</v>
@@ -18794,7 +18794,7 @@
         <v>70</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J89" s="11">
         <v>10</v>
@@ -18985,7 +18985,7 @@
         <v>70</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J90" s="11">
         <v>10</v>
@@ -19749,7 +19749,7 @@
         <v>70</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J94" s="11">
         <v>10</v>
@@ -19924,7 +19924,7 @@
         <v>70</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J95" s="11">
         <v>10</v>
@@ -20115,7 +20115,7 @@
         <v>70</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J96" s="11">
         <v>10</v>
@@ -20670,7 +20670,7 @@
         <v>70</v>
       </c>
       <c r="I99" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J99" s="11">
         <v>10</v>
@@ -20861,7 +20861,7 @@
         <v>70</v>
       </c>
       <c r="I100" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J100" s="11">
         <v>10</v>
@@ -21036,7 +21036,7 @@
         <v>70</v>
       </c>
       <c r="I101" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J101" s="11">
         <v>10</v>
@@ -21609,7 +21609,7 @@
         <v>70</v>
       </c>
       <c r="I104" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J104" s="11">
         <v>10</v>
@@ -21975,7 +21975,7 @@
         <v>70</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J106" s="11">
         <v>10</v>
@@ -22166,7 +22166,7 @@
         <v>70</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J107" s="11">
         <v>10</v>
@@ -22723,7 +22723,7 @@
         <v>70</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J110" s="11">
         <v>10</v>
@@ -23105,7 +23105,7 @@
         <v>70</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J112" s="11">
         <v>10</v>
@@ -23471,7 +23471,7 @@
         <v>70</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J114" s="11">
         <v>10</v>
@@ -23853,7 +23853,7 @@
         <v>70</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J116" s="11">
         <v>10</v>
@@ -24800,7 +24800,7 @@
         <v>70</v>
       </c>
       <c r="I121" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J121" s="11">
         <v>10</v>
@@ -24975,7 +24975,7 @@
         <v>70</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J122" s="11">
         <v>10</v>
@@ -25166,7 +25166,7 @@
         <v>70</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J123" s="11">
         <v>10</v>
@@ -25357,7 +25357,7 @@
         <v>70</v>
       </c>
       <c r="I124" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J124" s="11">
         <v>10</v>
@@ -25731,7 +25731,7 @@
         <v>70</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J126" s="11">
         <v>10</v>
@@ -26099,7 +26099,7 @@
         <v>70</v>
       </c>
       <c r="I128" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J128" s="11">
         <v>10</v>
@@ -26290,7 +26290,7 @@
         <v>70</v>
       </c>
       <c r="I129" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J129" s="11">
         <v>10</v>
@@ -26823,7 +26823,7 @@
         <v>70</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J132" s="11">
         <v>10</v>
@@ -27173,7 +27173,7 @@
         <v>70</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J134" s="11">
         <v>10</v>
@@ -27913,7 +27913,7 @@
         <v>70</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J138" s="11">
         <v>10</v>
@@ -28088,7 +28088,7 @@
         <v>70</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J139" s="11">
         <v>10</v>
@@ -28653,7 +28653,7 @@
         <v>70</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J142" s="11">
         <v>10</v>
@@ -28828,7 +28828,7 @@
         <v>70</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J143" s="11">
         <v>10</v>
@@ -29003,7 +29003,7 @@
         <v>70</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J144" s="11">
         <v>10</v>

</xml_diff>